<commit_message>
Dependency Injection ＆ Providers - 1 - Overview
</commit_message>
<xml_diff>
--- a/Sequence_To_Follow_Dependencies_Mapping.xlsx
+++ b/Sequence_To_Follow_Dependencies_Mapping.xlsx
@@ -1,13 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9E1AF9-6670-42D5-B515-A7C02C84D8F1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Quickstart - Nesting Components &amp; Inputs</t>
   </si>
@@ -40,12 +42,69 @@
   </si>
   <si>
     <t>Unit Testing - 4 - Testing with Mocks &amp; Spies</t>
+  </si>
+  <si>
+    <t>Module Category</t>
+  </si>
+  <si>
+    <t>Frequency to review so that we will not forget the contents</t>
+  </si>
+  <si>
+    <t>1.quickstart</t>
+  </si>
+  <si>
+    <t>2.es6-typescript</t>
+  </si>
+  <si>
+    <t>3.angular-cli</t>
+  </si>
+  <si>
+    <t>4.components</t>
+  </si>
+  <si>
+    <t>5.built-in-directives</t>
+  </si>
+  <si>
+    <t>6.custom-directives</t>
+  </si>
+  <si>
+    <t>7.reactive-programming-with-rxjs</t>
+  </si>
+  <si>
+    <t>Level of use in daily life</t>
+  </si>
+  <si>
+    <t>Basic/Intermediate/Expert</t>
+  </si>
+  <si>
+    <t>8.pipes</t>
+  </si>
+  <si>
+    <t>9.forms</t>
+  </si>
+  <si>
+    <t>10.dependency-injection-and-providers</t>
+  </si>
+  <si>
+    <t>11.HTTP</t>
+  </si>
+  <si>
+    <t>12.routing</t>
+  </si>
+  <si>
+    <t>13.unit-testing</t>
+  </si>
+  <si>
+    <t>14.advanced-topics</t>
+  </si>
+  <si>
+    <t>Your level of expertise</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -356,11 +415,121 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="33.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0CB7355-DA65-42C6-9951-4C97E5538E7F}">
   <dimension ref="B6:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>